<commit_message>
one point of setting and getting categories (contactdata)
</commit_message>
<xml_diff>
--- a/data/new.xlsx
+++ b/data/new.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2682,10 +2682,8 @@
       <c r="A39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="B39" t="n">
+        <v>6</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2702,42 +2700,280 @@
           <t>https://www.linkedin.com/in/alastair-stewart-187a5512</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Legal &amp; General</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Venture Capital</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2024-11-14 00:00:00</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Caucasian</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>40-49</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Finance/Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Fraser</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Thorne</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/fraser-thorne-57974510</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Edison Group</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Founder, CEO</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2024-11-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Caucasian</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>50-59</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Finance/Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Reiss</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Garwood</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/reiss-garwood-635b09b6</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>eXp Realty</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Independent property consultant</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2024-11-18 00:00:00</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Caucasian</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Finance/Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B42" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Jonny</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/jonny-page</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Esmée Fairbairn Foundation</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Head of Social and Impact Investment</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2024-11-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Caucasian</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Charity</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Douglas</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Sloan</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/in/douglassloan</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
         <is>
           <t>NaN</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Legal &amp; General</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Venture Capital</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2024-11-14 00:00:00</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>Caucasian</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>40-49</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>ImpactVC</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Co-Founder</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2024-11-15 00:00:00</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Caucasian</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>30-39</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
         <is>
           <t>Finance/Business</t>
         </is>

</xml_diff>